<commit_message>
fixes to excel export for bp report
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/BBBP-Challenge-Annual-Reporting-Form.xlsx
+++ b/src/assets/csv_templates/BBBP-Challenge-Annual-Reporting-Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/txr/dev/VERIFI/src/assets/csv_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4C7EA5-95FF-DF46-9A9C-99E7DACB7B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A8189C-0835-B943-BBA0-48EB89A6829F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="18080" windowHeight="19820" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="26460" windowHeight="19820" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -1889,21 +1889,43 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1916,30 +1938,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3980,7 +3980,7 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -3989,104 +3989,45 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>896470</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>212668</xdr:rowOff>
+      <xdr:colOff>900953</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>21665</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Text Box 2">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1040EBC-E7E6-0CB3-C96D-3FE2D017CA87}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="9424147" y="1008529"/>
-          <a:ext cx="1871382" cy="436786"/>
+          <a:off x="10802471" y="1030941"/>
+          <a:ext cx="2006600" cy="469900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rot="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" anchorCtr="0">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0">
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="1F497D"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>OMB Control No. 1910-5141</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:effectLst/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0">
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="1F497D"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>Exp. Date 6/30/2019</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:effectLst/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4843,20 +4784,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="70" customHeight="1">
-      <c r="A1" s="80"/>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+      <c r="A1" s="91"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" customHeight="1">
       <c r="A2" s="25"/>
@@ -4871,17 +4812,17 @@
       <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
       <c r="K3" s="78" t="s">
         <v>3</v>
       </c>
@@ -4893,437 +4834,437 @@
       <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="93"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="85"/>
     </row>
     <row r="5" spans="1:14" ht="46.5" customHeight="1">
       <c r="A5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="83"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="82"/>
     </row>
     <row r="6" spans="1:14" ht="46.5" customHeight="1">
       <c r="A6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="83"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="82"/>
     </row>
     <row r="7" spans="1:14" ht="46.5" customHeight="1">
       <c r="A7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="83"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="82"/>
     </row>
     <row r="8" spans="1:14" ht="46.5" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="83"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="82"/>
     </row>
     <row r="9" spans="1:14" ht="46.5" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="83"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="82"/>
     </row>
     <row r="10" spans="1:14" ht="46.5" customHeight="1">
       <c r="A10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="83"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="82"/>
     </row>
     <row r="11" spans="1:14" ht="46.5" customHeight="1">
       <c r="A11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
-      <c r="M11" s="82"/>
-      <c r="N11" s="83"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="82"/>
     </row>
     <row r="12" spans="1:14" ht="46.5" customHeight="1">
       <c r="A12" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="84"/>
-      <c r="M12" s="84"/>
-      <c r="N12" s="85"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="93"/>
     </row>
     <row r="13" spans="1:14" ht="46.5" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="83"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="82"/>
     </row>
     <row r="14" spans="1:14" ht="29.25" customHeight="1">
       <c r="A14" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="82"/>
-      <c r="M14" s="82"/>
-      <c r="N14" s="83"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="82"/>
     </row>
     <row r="15" spans="1:14" ht="36" customHeight="1">
       <c r="A15" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="89"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="96"/>
     </row>
     <row r="16" spans="1:14" ht="48" customHeight="1">
       <c r="A16" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="89"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="96"/>
     </row>
     <row r="17" spans="1:14" ht="46.5" customHeight="1">
       <c r="A17" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="88"/>
-      <c r="N17" s="88"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
     </row>
     <row r="18" spans="1:14" ht="46.5" customHeight="1">
       <c r="A18" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="84"/>
-      <c r="M18" s="84"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="92"/>
+      <c r="M18" s="92"/>
       <c r="N18" s="42"/>
     </row>
     <row r="19" spans="1:14" ht="64.5" customHeight="1">
       <c r="A19" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="88"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="88"/>
-      <c r="N19" s="88"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="87"/>
+      <c r="N19" s="87"/>
     </row>
     <row r="20" spans="1:14" ht="46.5" customHeight="1">
       <c r="A20" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="83"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="82"/>
     </row>
     <row r="21" spans="1:14" ht="46.5" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="82"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="82"/>
-      <c r="N21" s="83"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="81"/>
+      <c r="N21" s="82"/>
     </row>
     <row r="22" spans="1:14" ht="48" customHeight="1">
       <c r="A22" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="88" t="s">
+      <c r="B22" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="88"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="88"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="88"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
+      <c r="N22" s="87"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="88"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
+      <c r="N23" s="87"/>
     </row>
     <row r="24" spans="1:14" ht="83.25" customHeight="1">
-      <c r="A24" s="96"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="88"/>
-      <c r="M24" s="88"/>
-      <c r="N24" s="88"/>
+      <c r="A24" s="89"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
+      <c r="J24" s="87"/>
+      <c r="K24" s="87"/>
+      <c r="L24" s="87"/>
+      <c r="M24" s="87"/>
+      <c r="N24" s="87"/>
     </row>
     <row r="25" spans="1:14" ht="83.25" customHeight="1">
       <c r="A25" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="82"/>
-      <c r="L25" s="82"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="83"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="81"/>
+      <c r="J25" s="81"/>
+      <c r="K25" s="81"/>
+      <c r="L25" s="81"/>
+      <c r="M25" s="81"/>
+      <c r="N25" s="82"/>
     </row>
     <row r="26" spans="1:14" ht="16">
       <c r="A26" s="29"/>
@@ -5342,35 +5283,35 @@
       <c r="N26" s="30"/>
     </row>
     <row r="27" spans="1:14" ht="183" customHeight="1">
-      <c r="A27" s="94"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="94"/>
-      <c r="I27" s="94"/>
-      <c r="J27" s="94"/>
-      <c r="K27" s="94"/>
-      <c r="L27" s="94"/>
-      <c r="M27" s="94"/>
+      <c r="A27" s="86"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="86"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="86"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="86"/>
+      <c r="M27" s="86"/>
     </row>
     <row r="28" spans="1:14" ht="40" customHeight="1">
-      <c r="A28" s="90"/>
-      <c r="B28" s="90"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="90"/>
+      <c r="A28" s="79"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="79"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="79"/>
+      <c r="M28" s="79"/>
+      <c r="N28" s="79"/>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="31"/>
@@ -5404,18 +5345,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A28:N28"/>
-    <mergeCell ref="B8:N8"/>
-    <mergeCell ref="B9:N9"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="B6:N6"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="A27:M27"/>
-    <mergeCell ref="B22:N22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:N24"/>
-    <mergeCell ref="B25:N25"/>
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B21:N21"/>
@@ -5430,6 +5359,18 @@
     <mergeCell ref="B18:M18"/>
     <mergeCell ref="B19:N19"/>
     <mergeCell ref="B20:N20"/>
+    <mergeCell ref="A28:N28"/>
+    <mergeCell ref="B8:N8"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="B22:N22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:N24"/>
+    <mergeCell ref="B25:N25"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.25" bottom="0.25" header="0" footer="0"/>
@@ -5445,8 +5386,8 @@
   </sheetPr>
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="25" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="25" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fix rounding issue in reports and summation in excel BP report
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/BBBP-Challenge-Annual-Reporting-Form.xlsx
+++ b/src/assets/csv_templates/BBBP-Challenge-Annual-Reporting-Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/txr/Documents/VERIFI-Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/txr/dev/VERIFI/src/assets/csv_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7524D6A1-E072-8744-9AE3-99E26B99B4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39287B4-BB8B-2C48-BDB2-9324E087E95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="22620" windowHeight="19820" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="22620" windowHeight="19720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -1889,7 +1889,12 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1899,6 +1904,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1911,35 +1935,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4784,20 +4784,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="70" customHeight="1">
-      <c r="A1" s="91"/>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" customHeight="1">
       <c r="A2" s="25"/>
@@ -4812,17 +4812,17 @@
       <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
       <c r="K3" s="78" t="s">
         <v>3</v>
       </c>
@@ -4834,437 +4834,437 @@
       <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="85"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="92"/>
+      <c r="N4" s="93"/>
     </row>
     <row r="5" spans="1:14" ht="46.5" customHeight="1">
       <c r="A5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="82"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="83"/>
     </row>
     <row r="6" spans="1:14" ht="46.5" customHeight="1">
       <c r="A6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="83"/>
     </row>
     <row r="7" spans="1:14" ht="46.5" customHeight="1">
       <c r="A7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="83"/>
     </row>
     <row r="8" spans="1:14" ht="46.5" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="83"/>
     </row>
     <row r="9" spans="1:14" ht="46.5" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="83"/>
     </row>
     <row r="10" spans="1:14" ht="46.5" customHeight="1">
       <c r="A10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="83"/>
     </row>
     <row r="11" spans="1:14" ht="46.5" customHeight="1">
       <c r="A11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="83"/>
     </row>
     <row r="12" spans="1:14" ht="46.5" customHeight="1">
       <c r="A12" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="93"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="84"/>
+      <c r="L12" s="84"/>
+      <c r="M12" s="84"/>
+      <c r="N12" s="85"/>
     </row>
     <row r="13" spans="1:14" ht="46.5" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="83"/>
     </row>
     <row r="14" spans="1:14" ht="29.25" customHeight="1">
       <c r="A14" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="83"/>
     </row>
     <row r="15" spans="1:14" ht="36" customHeight="1">
       <c r="A15" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="96"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="89"/>
     </row>
     <row r="16" spans="1:14" ht="48" customHeight="1">
       <c r="A16" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="96"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="88"/>
+      <c r="G16" s="88"/>
+      <c r="H16" s="88"/>
+      <c r="I16" s="88"/>
+      <c r="J16" s="88"/>
+      <c r="K16" s="88"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="88"/>
+      <c r="N16" s="89"/>
     </row>
     <row r="17" spans="1:14" ht="46.5" customHeight="1">
       <c r="A17" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="88"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="88"/>
+      <c r="N17" s="88"/>
     </row>
     <row r="18" spans="1:14" ht="46.5" customHeight="1">
       <c r="A18" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="92"/>
-      <c r="M18" s="92"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="84"/>
+      <c r="L18" s="84"/>
+      <c r="M18" s="84"/>
       <c r="N18" s="42"/>
     </row>
     <row r="19" spans="1:14" ht="64.5" customHeight="1">
       <c r="A19" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="87"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="87"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88"/>
+      <c r="N19" s="88"/>
     </row>
     <row r="20" spans="1:14" ht="46.5" customHeight="1">
       <c r="A20" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="94" t="s">
+      <c r="B20" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="82"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="83"/>
     </row>
     <row r="21" spans="1:14" ht="46.5" customHeight="1">
       <c r="A21" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="82"/>
+      <c r="N21" s="83"/>
     </row>
     <row r="22" spans="1:14" ht="48" customHeight="1">
       <c r="A22" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="87"/>
-      <c r="N22" s="87"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
+      <c r="H22" s="88"/>
+      <c r="I22" s="88"/>
+      <c r="J22" s="88"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="88"/>
+      <c r="N22" s="88"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1">
-      <c r="A23" s="88" t="s">
+      <c r="A23" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="87"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="88"/>
+      <c r="K23" s="88"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="88"/>
+      <c r="N23" s="88"/>
     </row>
     <row r="24" spans="1:14" ht="83.25" customHeight="1">
-      <c r="A24" s="89"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="87"/>
+      <c r="A24" s="96"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
     </row>
     <row r="25" spans="1:14" ht="83.25" customHeight="1">
       <c r="A25" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="81" t="s">
+      <c r="B25" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="81"/>
-      <c r="J25" s="81"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="81"/>
-      <c r="M25" s="81"/>
-      <c r="N25" s="82"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="83"/>
     </row>
     <row r="26" spans="1:14" ht="16">
       <c r="A26" s="29"/>
@@ -5283,35 +5283,35 @@
       <c r="N26" s="30"/>
     </row>
     <row r="27" spans="1:14" ht="183" customHeight="1">
-      <c r="A27" s="86"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="86"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="86"/>
-      <c r="K27" s="86"/>
-      <c r="L27" s="86"/>
-      <c r="M27" s="86"/>
+      <c r="A27" s="94"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="94"/>
+      <c r="J27" s="94"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="94"/>
+      <c r="M27" s="94"/>
     </row>
     <row r="28" spans="1:14" ht="40" customHeight="1">
-      <c r="A28" s="79"/>
-      <c r="B28" s="79"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="79"/>
+      <c r="A28" s="90"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="31"/>
@@ -5345,6 +5345,18 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A28:N28"/>
+    <mergeCell ref="B8:N8"/>
+    <mergeCell ref="B9:N9"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="B22:N22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:N24"/>
+    <mergeCell ref="B25:N25"/>
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B21:N21"/>
@@ -5359,18 +5371,6 @@
     <mergeCell ref="B18:M18"/>
     <mergeCell ref="B19:N19"/>
     <mergeCell ref="B20:N20"/>
-    <mergeCell ref="A28:N28"/>
-    <mergeCell ref="B8:N8"/>
-    <mergeCell ref="B9:N9"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="B6:N6"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="A27:M27"/>
-    <mergeCell ref="B22:N22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:N24"/>
-    <mergeCell ref="B25:N25"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.25" bottom="0.25" header="0" footer="0"/>
@@ -5387,7 +5387,7 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="25" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6306,11 +6306,11 @@
         <v>61</v>
       </c>
       <c r="D26" s="21">
-        <f>SUM(D14:D24)</f>
+        <f>SUM(D14:D25)</f>
         <v>0</v>
       </c>
       <c r="E26" s="21">
-        <f>SUM(E14:E24)</f>
+        <f>SUM(E14:E25)</f>
         <v>0</v>
       </c>
       <c r="F26" s="46"/>

</xml_diff>